<commit_message>
Created Data's Descriptive Statistics
</commit_message>
<xml_diff>
--- a/excel/descriptive-statistics-in-excel/coffee_sales_descriptive_statistics.xlsx
+++ b/excel/descriptive-statistics-in-excel/coffee_sales_descriptive_statistics.xlsx
@@ -8,24 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\OLAITAN-PC\Documents\Career\Projects\mini-projects\excel\descriptive-statistics-in-excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F3E4E741-655E-46B9-B9C1-77B7B220E04B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B1C754-9031-4113-8C3F-B8352D290A08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="285" windowWidth="20730" windowHeight="10905" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="20370" yWindow="285" windowWidth="24240" windowHeight="12885" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="33">
   <si>
     <t>City</t>
   </si>
@@ -85,13 +94,52 @@
   </si>
   <si>
     <t>New York</t>
+  </si>
+  <si>
+    <t>Mean</t>
+  </si>
+  <si>
+    <t>Standard Error</t>
+  </si>
+  <si>
+    <t>Median</t>
+  </si>
+  <si>
+    <t>Mode</t>
+  </si>
+  <si>
+    <t>Standard Deviation</t>
+  </si>
+  <si>
+    <t>Sample Variance</t>
+  </si>
+  <si>
+    <t>Kurtosis</t>
+  </si>
+  <si>
+    <t>Skewness</t>
+  </si>
+  <si>
+    <t>Range</t>
+  </si>
+  <si>
+    <t>Minimum</t>
+  </si>
+  <si>
+    <t>Maximum</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Count</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,16 +147,58 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -116,20 +206,126 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="centerContinuous"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="5">
     <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="1" tint="0.249977111117893"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
       <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -148,16 +344,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>438149</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>47625</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>438150</xdr:colOff>
       <xdr:row>3</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>138112</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -172,8 +368,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="304800" y="247650"/>
-          <a:ext cx="2924175" cy="457200"/>
+          <a:off x="1047749" y="385762"/>
+          <a:ext cx="1581151" cy="323850"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -203,22 +399,113 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-GB" sz="1800">
-              <a:latin typeface="Abhaya Libre" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cooper Black" panose="0208090404030B020404" pitchFamily="18" charset="0"/>
               <a:cs typeface="Abhaya Libre" panose="02000503000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
-            <a:t>Coffe</a:t>
+            <a:t>Coffee</a:t>
           </a:r>
           <a:r>
             <a:rPr lang="en-GB" sz="1800" baseline="0">
-              <a:latin typeface="Abhaya Libre" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cooper Black" panose="0208090404030B020404" pitchFamily="18" charset="0"/>
               <a:cs typeface="Abhaya Libre" panose="02000503000000000000" pitchFamily="2" charset="0"/>
             </a:rPr>
-            <a:t> Sales Sample Dataset</a:t>
+            <a:t> Sales</a:t>
           </a:r>
           <a:endParaRPr lang="en-GB" sz="1800">
-            <a:latin typeface="Abhaya Libre" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="75000"/>
+                <a:lumOff val="25000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:latin typeface="Cooper Black" panose="0208090404030B020404" pitchFamily="18" charset="0"/>
             <a:cs typeface="Abhaya Libre" panose="02000503000000000000" pitchFamily="2" charset="0"/>
           </a:endParaRPr>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>161924</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>4762</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>428625</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>138112</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EAA12DF1-53D3-4816-BD28-47498940E7A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4981574" y="385762"/>
+          <a:ext cx="2695576" cy="323850"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1800">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="75000"/>
+                  <a:lumOff val="25000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="Cooper Black" panose="0208090404030B020404" pitchFamily="18" charset="0"/>
+              <a:cs typeface="Abhaya Libre" panose="02000503000000000000" pitchFamily="2" charset="0"/>
+            </a:rPr>
+            <a:t>Descriptive Statistics</a:t>
+          </a:r>
         </a:p>
       </xdr:txBody>
     </xdr:sp>
@@ -228,14 +515,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C6BFDC37-0C62-4858-B014-7673609C8C62}" name="Table1" displayName="Table1" ref="B5:D65" totalsRowShown="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{C6BFDC37-0C62-4858-B014-7673609C8C62}" name="Table1" displayName="Table1" ref="B5:D65" totalsRowShown="0" headerRowDxfId="0" dataDxfId="4">
   <autoFilter ref="B5:D65" xr:uid="{C6BFDC37-0C62-4858-B014-7673609C8C62}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{80EFC2C1-D69E-43D4-856F-56DFFD3FF353}" name="City"/>
-    <tableColumn id="2" xr3:uid="{856228B2-8A1F-4FB5-BF0B-9EF3286344D9}" name="Month"/>
-    <tableColumn id="3" xr3:uid="{F20AB32B-712D-4107-8954-D5EC99637F0D}" name=" Sales " dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{80EFC2C1-D69E-43D4-856F-56DFFD3FF353}" name="City" dataDxfId="3"/>
+    <tableColumn id="2" xr3:uid="{856228B2-8A1F-4FB5-BF0B-9EF3286344D9}" name="Month" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{F20AB32B-712D-4107-8954-D5EC99637F0D}" name=" Sales " dataDxfId="1"/>
   </tableColumns>
-  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+  <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
@@ -502,695 +789,783 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B5:D65"/>
+  <dimension ref="B4:K65"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="11.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.85546875" customWidth="1"/>
+    <col min="3" max="3" width="9.85546875" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
+    <col min="9" max="9" width="18.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="4" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="5" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="4" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="I5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="J5" s="5"/>
+    </row>
+    <row r="6" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D6" s="1">
+      <c r="D6" s="2">
         <v>41362</v>
       </c>
-    </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="1">
+      <c r="D7" s="2">
         <v>41466</v>
       </c>
-    </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
+      <c r="I7" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="J7" s="7">
+        <v>46105.583333333336</v>
+      </c>
+    </row>
+    <row r="8" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="1">
+      <c r="D8" s="2">
         <v>42021</v>
       </c>
-    </row>
-    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
+      <c r="I8" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="J8" s="6">
+        <v>383.17219085993082</v>
+      </c>
+    </row>
+    <row r="9" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="1">
+      <c r="D9" s="2">
         <v>42130</v>
       </c>
-    </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
+      <c r="I9" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="J9" s="7">
+        <v>45860</v>
+      </c>
+    </row>
+    <row r="10" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B10" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D10" s="1">
+      <c r="D10" s="2">
         <v>42130</v>
       </c>
-    </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
+      <c r="I10" s="6" t="s">
+        <v>23</v>
+      </c>
+      <c r="J10" s="6">
+        <v>42130</v>
+      </c>
+    </row>
+    <row r="11" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B11" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="1">
+      <c r="D11" s="2">
         <v>42140</v>
       </c>
-    </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
+      <c r="I11" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="J11" s="7">
+        <v>2968.0390278606437</v>
+      </c>
+    </row>
+    <row r="12" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="1">
+      <c r="D12" s="2">
         <v>42267</v>
       </c>
-    </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
+      <c r="I12" s="6" t="s">
+        <v>25</v>
+      </c>
+      <c r="J12" s="6">
+        <v>8809255.6709039547</v>
+      </c>
+      <c r="K12" s="3"/>
+    </row>
+    <row r="13" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B13" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="1">
+      <c r="D13" s="2">
         <v>42354</v>
       </c>
-    </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
+      <c r="I13" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="J13" s="7">
+        <v>-1.1506836524955388</v>
+      </c>
+    </row>
+    <row r="14" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B14" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D14" s="1">
+      <c r="D14" s="2">
         <v>42474</v>
       </c>
-    </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B15" t="s">
+      <c r="I14" s="6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J14" s="6">
+        <v>0.21595921248962099</v>
+      </c>
+    </row>
+    <row r="15" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B15" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D15" s="1">
+      <c r="D15" s="2">
         <v>42685</v>
       </c>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B16" t="s">
+      <c r="I15" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="J15" s="7">
+        <v>10018</v>
+      </c>
+    </row>
+    <row r="16" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D16" s="1">
+      <c r="D16" s="2">
         <v>42955</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B17" t="s">
+      <c r="I16" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="J16" s="6">
+        <v>41362</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C17" t="s">
+      <c r="C17" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D17" s="1">
+      <c r="D17" s="2">
         <v>43189</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B18" t="s">
+      <c r="I17" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="J17" s="7">
+        <v>51380</v>
+      </c>
+    </row>
+    <row r="18" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C18" t="s">
+      <c r="C18" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D18" s="1">
+      <c r="D18" s="2">
         <v>43294</v>
       </c>
-    </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="I18" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="J18" s="6">
+        <v>2766335</v>
+      </c>
+    </row>
+    <row r="19" spans="2:10" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C19" t="s">
+      <c r="C19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="1">
+      <c r="D19" s="2">
         <v>43515</v>
       </c>
-    </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" t="s">
+      <c r="I19" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="J19" s="8">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C20" t="s">
+      <c r="C20" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D20" s="1">
+      <c r="D20" s="2">
         <v>43734</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" t="s">
+    <row r="21" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B21" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C21" t="s">
+      <c r="C21" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D21" s="1">
+      <c r="D21" s="2">
         <v>43747</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B22" t="s">
+    <row r="22" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C22" t="s">
+      <c r="C22" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D22" s="1">
+      <c r="D22" s="2">
         <v>43888</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
+    <row r="23" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B23" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C23" t="s">
+      <c r="C23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D23" s="1">
+      <c r="D23" s="2">
         <v>44068</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" t="s">
+    <row r="24" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B24" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C24" t="s">
+      <c r="C24" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="1">
+      <c r="D24" s="2">
         <v>44135</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
+    <row r="25" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B25" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C25" t="s">
+      <c r="C25" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D25" s="1">
+      <c r="D25" s="2">
         <v>44169</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
+    <row r="26" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B26" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C26" t="s">
+      <c r="C26" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D26" s="1">
+      <c r="D26" s="2">
         <v>44215</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
+    <row r="27" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B27" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C27" t="s">
+      <c r="C27" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="1">
+      <c r="D27" s="2">
         <v>44444</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B28" t="s">
+    <row r="28" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B28" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C28" t="s">
+      <c r="C28" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="1">
+      <c r="D28" s="2">
         <v>44482</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B29" t="s">
+    <row r="29" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B29" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C29" t="s">
+      <c r="C29" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="1">
+      <c r="D29" s="2">
         <v>44485</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
+    <row r="30" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B30" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C30" t="s">
+      <c r="C30" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D30" s="1">
+      <c r="D30" s="2">
         <v>44899</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B31" t="s">
+    <row r="31" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B31" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C31" t="s">
+      <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D31" s="1">
+      <c r="D31" s="2">
         <v>45005</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B32" t="s">
+    <row r="32" spans="2:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B32" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D32" s="1">
+      <c r="D32" s="2">
         <v>45047</v>
       </c>
     </row>
-    <row r="33" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
+    <row r="33" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B33" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C33" t="s">
+      <c r="C33" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D33" s="1">
+      <c r="D33" s="2">
         <v>45391</v>
       </c>
     </row>
-    <row r="34" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B34" t="s">
+    <row r="34" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B34" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C34" t="s">
+      <c r="C34" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D34" s="1">
+      <c r="D34" s="2">
         <v>45547</v>
       </c>
     </row>
-    <row r="35" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B35" t="s">
+    <row r="35" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B35" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C35" t="s">
+      <c r="C35" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D35" s="1">
+      <c r="D35" s="2">
         <v>45638</v>
       </c>
     </row>
-    <row r="36" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+    <row r="36" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B36" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C36" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D36" s="1">
+      <c r="D36" s="2">
         <v>46082</v>
       </c>
     </row>
-    <row r="37" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B37" t="s">
+    <row r="37" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C37" t="s">
+      <c r="C37" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D37" s="1">
+      <c r="D37" s="2">
         <v>46330</v>
       </c>
     </row>
-    <row r="38" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B38" t="s">
+    <row r="38" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B38" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C38" t="s">
+      <c r="C38" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D38" s="1">
+      <c r="D38" s="2">
         <v>46385</v>
       </c>
     </row>
-    <row r="39" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B39" t="s">
+    <row r="39" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B39" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C39" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D39" s="1">
+      <c r="D39" s="2">
         <v>46459</v>
       </c>
     </row>
-    <row r="40" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
+    <row r="40" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B40" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C40" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D40" s="1">
+      <c r="D40" s="2">
         <v>46562</v>
       </c>
     </row>
-    <row r="41" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B41" t="s">
+    <row r="41" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B41" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C41" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D41" s="1">
+      <c r="D41" s="2">
         <v>46632</v>
       </c>
     </row>
-    <row r="42" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B42" t="s">
+    <row r="42" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B42" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C42" t="s">
+      <c r="C42" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D42" s="1">
+      <c r="D42" s="2">
         <v>46735</v>
       </c>
     </row>
-    <row r="43" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B43" t="s">
+    <row r="43" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B43" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C43" t="s">
+      <c r="C43" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D43" s="1">
+      <c r="D43" s="2">
         <v>46769</v>
       </c>
     </row>
-    <row r="44" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B44" t="s">
+    <row r="44" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B44" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C44" t="s">
+      <c r="C44" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D44" s="1">
+      <c r="D44" s="2">
         <v>47300</v>
       </c>
     </row>
-    <row r="45" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B45" t="s">
+    <row r="45" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B45" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C45" t="s">
+      <c r="C45" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D45" s="2">
         <v>47324</v>
       </c>
     </row>
-    <row r="46" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B46" t="s">
+    <row r="46" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B46" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D46" s="1">
+      <c r="D46" s="2">
         <v>47528</v>
       </c>
     </row>
-    <row r="47" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B47" t="s">
+    <row r="47" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B47" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C47" t="s">
+      <c r="C47" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="1">
+      <c r="D47" s="2">
         <v>47806</v>
       </c>
     </row>
-    <row r="48" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B48" t="s">
+    <row r="48" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B48" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D48" s="1">
+      <c r="D48" s="2">
         <v>48433</v>
       </c>
     </row>
-    <row r="49" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B49" t="s">
+    <row r="49" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B49" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C49" t="s">
+      <c r="C49" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D49" s="1">
+      <c r="D49" s="2">
         <v>48747</v>
       </c>
     </row>
-    <row r="50" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B50" t="s">
+    <row r="50" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B50" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C50" t="s">
+      <c r="C50" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D50" s="1">
+      <c r="D50" s="2">
         <v>48904</v>
       </c>
     </row>
-    <row r="51" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B51" t="s">
+    <row r="51" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B51" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D51" s="1">
+      <c r="D51" s="2">
         <v>48919</v>
       </c>
     </row>
-    <row r="52" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B52" t="s">
+    <row r="52" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B52" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D52" s="1">
+      <c r="D52" s="2">
         <v>48975</v>
       </c>
     </row>
-    <row r="53" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B53" t="s">
+    <row r="53" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B53" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C53" t="s">
+      <c r="C53" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D53" s="1">
+      <c r="D53" s="2">
         <v>49095</v>
       </c>
     </row>
-    <row r="54" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B54" t="s">
+    <row r="54" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B54" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C54" t="s">
+      <c r="C54" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D54" s="1">
+      <c r="D54" s="2">
         <v>49184</v>
       </c>
     </row>
-    <row r="55" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B55" t="s">
+    <row r="55" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B55" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C55" t="s">
+      <c r="C55" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="D55" s="1">
+      <c r="D55" s="2">
         <v>49238</v>
       </c>
     </row>
-    <row r="56" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B56" t="s">
+    <row r="56" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B56" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C56" t="s">
+      <c r="C56" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D56" s="1">
+      <c r="D56" s="2">
         <v>49507</v>
       </c>
     </row>
-    <row r="57" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B57" t="s">
+    <row r="57" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B57" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C57" t="s">
+      <c r="C57" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D57" s="1">
+      <c r="D57" s="2">
         <v>49753</v>
       </c>
     </row>
-    <row r="58" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B58" t="s">
+    <row r="58" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B58" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C58" t="s">
+      <c r="C58" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D58" s="1">
+      <c r="D58" s="2">
         <v>49772</v>
       </c>
     </row>
-    <row r="59" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B59" t="s">
+    <row r="59" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B59" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C59" t="s">
+      <c r="C59" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="D59" s="1">
+      <c r="D59" s="2">
         <v>50558</v>
       </c>
     </row>
-    <row r="60" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B60" t="s">
+    <row r="60" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B60" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C60" t="s">
+      <c r="C60" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D60" s="1">
+      <c r="D60" s="2">
         <v>50853</v>
       </c>
     </row>
-    <row r="61" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+    <row r="61" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B61" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C61" t="s">
+      <c r="C61" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D61" s="1">
+      <c r="D61" s="2">
         <v>50879</v>
       </c>
     </row>
-    <row r="62" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B62" t="s">
+    <row r="62" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B62" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C62" t="s">
+      <c r="C62" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D62" s="1">
+      <c r="D62" s="2">
         <v>51005</v>
       </c>
     </row>
-    <row r="63" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B63" t="s">
+    <row r="63" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B63" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C63" t="s">
+      <c r="C63" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D63" s="1">
+      <c r="D63" s="2">
         <v>51171</v>
       </c>
     </row>
-    <row r="64" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B64" t="s">
+    <row r="64" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B64" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C64" t="s">
+      <c r="C64" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D64" s="1">
+      <c r="D64" s="2">
         <v>51174</v>
       </c>
     </row>
-    <row r="65" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B65" t="s">
+    <row r="65" spans="2:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="B65" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C65" t="s">
+      <c r="C65" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D65" s="1">
+      <c r="D65" s="2">
         <v>51380</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>